<commit_message>
Test data updated 2
</commit_message>
<xml_diff>
--- a/JavaPrograms/TestDataSheet.xlsx
+++ b/JavaPrograms/TestDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179C0AA5-1E96-4390-9F8E-A1AB7518141F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50BF5CB-AFF4-46FF-A3D0-ED5EA3BD10BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Testdata1</t>
+  </si>
+  <si>
+    <t>TestData2</t>
   </si>
 </sst>
 </file>
@@ -340,15 +343,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test data updated 5
</commit_message>
<xml_diff>
--- a/JavaPrograms/TestDataSheet.xlsx
+++ b/JavaPrograms/TestDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7386995-A99B-4EB7-B8BF-3D4734B7EC45}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85ABADF-5B64-49E7-AFC5-02C15FF36643}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Testdata1</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Testdata3</t>
+  </si>
+  <si>
+    <t>Testdtata4</t>
   </si>
 </sst>
 </file>
@@ -346,15 +349,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -364,6 +367,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>